<commit_message>
Se añade tabla dimensional base (master)
</commit_message>
<xml_diff>
--- a/Webscrapping/Fuentes de datos Web Scrapping.xlsx
+++ b/Webscrapping/Fuentes de datos Web Scrapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto Web Scrapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto Web Scrapping\Webscrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51FB58D4-DD96-4F60-8DEF-812E179C3671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAFFCCF-307E-47DA-9F01-3E1D38AFD15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
+    <workbookView xWindow="6468" yWindow="12" windowWidth="16560" windowHeight="12216" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
   <si>
     <t>Marca</t>
   </si>
@@ -154,9 +153,6 @@
     <t>https://www.falabella.com.co/falabella-co/product/128906319/Celular-Samsung-Galaxy-A25-5G-256GB-8RAM+-Cargador/128906321</t>
   </si>
   <si>
-    <t>Samsung Galaxy A25 5G 256GB 8RAM</t>
-  </si>
-  <si>
     <t>https://www.falabella.com.co/falabella-co/product/129554425/Celular-Samsung-Galaxy-A55-5G-256Gb-8Ram-Azul-Oscuro/129554428</t>
   </si>
   <si>
@@ -176,6 +172,75 @@
   </si>
   <si>
     <t xml:space="preserve">Xiaomi Redmi Note 13 </t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A25</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung Galaxy A15 </t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/131931272/Celular-SAMSUNG-GALAXY-A25-256GB-+-8-RAM-AZUL-CLARO/131931273</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/72899217/Celular-Samsung-Galaxy-A35-5G-256GB-8GB-RAM-camara-posterior-50-MP-camara-frontal-13MP-pantalla-6.6-Pulgadas-+-Exynos-1380/72899217</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A35</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/128668464/Celular-Samsung-Galaxy-A05S-128Gb-Negro/128668465</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/133744591/Celular-Samsung-Galaxy-A35-256Gb-5g-Lila/133744592</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A05</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/128035979/Samsung-S24-Ultra-256GB-12GB-Violet/128035980</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/128853893/Celular-Samsung-Galaxy-S24-Ultra-De-256GB12GB-RAM-Gris-5G/128853894</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/129574090/Samsung-Galaxy-S24-Ultra-512GB-12GB-Ram-5G-Violeta/129574091</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/prod12000048/iPhone-13-128-GB-5G-4GB-RAM-Pantalla-6.1-Pulgadas-Chip-A15-Bionic/19604508</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung S24 Ultra </t>
+  </si>
+  <si>
+    <t>IPhone 13</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/prod13430667/iPhone-15-de-128GB-5G-6GB-RAM-Pantalla-6.1-pulgadas-Chip-A16-Bionic-Carga-Tipo-C-Dynamic-Island-Camara-48MP/72752105</t>
+  </si>
+  <si>
+    <t>IPhone 14</t>
+  </si>
+  <si>
+    <t>IPhone 15</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/prod13070047/iPhone-14-128GB-5G-6GB-RAM-Pantalla-6.1-Pulgadas-Chip-A15-Bionic-/60999138</t>
+  </si>
+  <si>
+    <t>https://www.falabella.com.co/falabella-co/product/prod10900027/iPhone-11-128-GB-4GB-RAM-Pantalla-6.1-Pulgadas-Chip-A13-Bionic-Camara-12-MP/9722720</t>
+  </si>
+  <si>
+    <t>IPhone 11</t>
   </si>
 </sst>
 </file>
@@ -234,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -242,6 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -522,13 +588,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:D25" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D25" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:F32" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F32" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{377E1240-9D46-430C-803F-4C08BD63303F}" name="Enlace" dataCellStyle="Hipervínculo"/>
     <tableColumn id="2" xr3:uid="{5FAAC6E1-7190-422A-92D1-B8DCED044495}" name="Sitio Web"/>
     <tableColumn id="3" xr3:uid="{6C7078F4-6973-409E-B572-0FE355E1A626}" name="Marca"/>
     <tableColumn id="4" xr3:uid="{8115CCF5-4C7A-4227-90FA-D41A410A4833}" name="Modelo"/>
+    <tableColumn id="5" xr3:uid="{F4F4B18E-B1F0-473E-AB7B-805E74619B4C}" name="Precio"/>
+    <tableColumn id="6" xr3:uid="{EE9A1EB6-30CC-48F5-816C-80D20CB21E97}" name="Código"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,18 +919,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8500B94C-5AFD-412C-8663-C5BE5B0FA223}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -875,8 +943,14 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -887,10 +961,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>1899900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -901,10 +978,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>1449900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -915,10 +995,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2199900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -929,10 +1012,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2199900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -943,10 +1029,13 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3099700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -957,10 +1046,13 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -971,10 +1063,13 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -985,10 +1080,13 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E9" s="5">
+        <v>879900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -999,10 +1097,13 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="E10" s="5">
+        <v>879900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1013,10 +1114,13 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E11" s="5">
+        <v>949900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1027,10 +1131,13 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1299900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1041,10 +1148,13 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1079900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1055,23 +1165,32 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="E14" s="5">
+        <v>669900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2499900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -1082,10 +1201,13 @@
       <c r="D16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="5">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -1094,12 +1216,15 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="E17" s="5">
+        <v>699900</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -1108,12 +1233,15 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="E18" s="5">
+        <v>612900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1122,12 +1250,15 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="E19" s="5">
+        <v>599900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1136,12 +1267,15 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="E20" s="5">
+        <v>612900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1150,12 +1284,15 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1235000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1164,11 +1301,16 @@
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1199900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -1176,25 +1318,163 @@
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="E23" s="5">
+        <v>969900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1299900</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="5">
+        <v>449900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="5">
+        <v>7500000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="5">
+        <v>7500000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="5">
+        <v>7499990</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="5">
+        <v>2799900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="5">
+        <v>3759900</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="5">
+        <v>3199900</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="5">
+        <v>2549900</v>
       </c>
     </row>
   </sheetData>
@@ -1213,17 +1493,28 @@
     <hyperlink ref="A12" r:id="rId11" xr:uid="{090E4DF1-D4C3-40CD-921A-453EF53FD8C2}"/>
     <hyperlink ref="A13" r:id="rId12" xr:uid="{9B0B241E-2775-4049-9C58-DFE1303229AC}"/>
     <hyperlink ref="A14" r:id="rId13" xr:uid="{B4E566C2-E281-4E14-85EF-0017A6237ED7}"/>
-    <hyperlink ref="A17" r:id="rId14" xr:uid="{7D27F7E4-07C5-4486-A09D-914A0DB4CBE6}"/>
-    <hyperlink ref="A18" r:id="rId15" xr:uid="{D1B444DD-33A9-498D-B3A9-9089A761661B}"/>
-    <hyperlink ref="A19" r:id="rId16" xr:uid="{3EAEB76C-F201-47A4-8325-1248E769E333}"/>
-    <hyperlink ref="A20" r:id="rId17" xr:uid="{98A5927C-997C-4285-9C5C-07EFD99C107A}"/>
-    <hyperlink ref="A21" r:id="rId18" xr:uid="{8CDECC3D-DA84-4D6E-B8CD-6915D1937740}"/>
-    <hyperlink ref="A22" r:id="rId19" xr:uid="{2D2B0672-EC1C-4184-8E98-33DEFC7FCED5}"/>
-    <hyperlink ref="A16" r:id="rId20" xr:uid="{BDDB22E4-BCCD-43FD-B377-4C9ACC77A8DC}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{7D27F7E4-07C5-4486-A09D-914A0DB4CBE6}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{D1B444DD-33A9-498D-B3A9-9089A761661B}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{3EAEB76C-F201-47A4-8325-1248E769E333}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{98A5927C-997C-4285-9C5C-07EFD99C107A}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{8CDECC3D-DA84-4D6E-B8CD-6915D1937740}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{2D2B0672-EC1C-4184-8E98-33DEFC7FCED5}"/>
+    <hyperlink ref="A15" r:id="rId20" xr:uid="{BDDB22E4-BCCD-43FD-B377-4C9ACC77A8DC}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{82270B06-9912-4791-97A1-C0EDDFBB60DF}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{F2382336-A0CF-4933-93E7-92BC97C63F56}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{EBE7E398-1E23-4786-83D7-6B064E34B571}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{3FFA4EF1-06AB-42C1-BE08-0BC48AA24A12}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{7E4554B0-87E3-4A1E-BDFF-155340CBA46C}"/>
+    <hyperlink ref="A27" r:id="rId26" xr:uid="{AE68D55E-9520-48FB-84C6-3EFEDBB73037}"/>
+    <hyperlink ref="A28" r:id="rId27" xr:uid="{7FA50F87-3340-48F3-B2EF-C56E5709038E}"/>
+    <hyperlink ref="A29" r:id="rId28" xr:uid="{0A62AC0B-84C1-43DA-86E7-84765FF424BF}"/>
+    <hyperlink ref="A30" r:id="rId29" xr:uid="{426D4B11-FA7E-4CD4-8D0B-95237D52D2DE}"/>
+    <hyperlink ref="A31" r:id="rId30" xr:uid="{354F6FE1-0A02-4D1D-A1B5-FDB8EED61F95}"/>
+    <hyperlink ref="A32" r:id="rId31" xr:uid="{662B402D-4086-4B7C-9655-FEA5DE28A50D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Se corrigió tabla master
</commit_message>
<xml_diff>
--- a/Webscrapping/Fuentes de datos Web Scrapping.xlsx
+++ b/Webscrapping/Fuentes de datos Web Scrapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto Web Scrapping\Webscrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAFFCCF-307E-47DA-9F01-3E1D38AFD15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0549A136-21AF-4B39-937D-BD4CB597311A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6468" yWindow="12" windowWidth="16560" windowHeight="12216" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="98">
   <si>
     <t>Marca</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Precio</t>
   </si>
   <si>
-    <t>Código</t>
-  </si>
-  <si>
     <t xml:space="preserve">Samsung Galaxy A15 </t>
   </si>
   <si>
@@ -241,6 +238,102 @@
   </si>
   <si>
     <t>IPhone 11</t>
+  </si>
+  <si>
+    <t>FX1</t>
+  </si>
+  <si>
+    <t>FX2</t>
+  </si>
+  <si>
+    <t>FX3</t>
+  </si>
+  <si>
+    <t>FX4</t>
+  </si>
+  <si>
+    <t>FX5</t>
+  </si>
+  <si>
+    <t>FS1</t>
+  </si>
+  <si>
+    <t>FS2</t>
+  </si>
+  <si>
+    <t>FS3</t>
+  </si>
+  <si>
+    <t>FS4</t>
+  </si>
+  <si>
+    <t>FS5</t>
+  </si>
+  <si>
+    <t>FS6</t>
+  </si>
+  <si>
+    <t>FI1</t>
+  </si>
+  <si>
+    <t>FI2</t>
+  </si>
+  <si>
+    <t>FI3</t>
+  </si>
+  <si>
+    <t>FI4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código </t>
+  </si>
+  <si>
+    <t>FX6</t>
+  </si>
+  <si>
+    <t>FX7</t>
+  </si>
+  <si>
+    <t>FX8</t>
+  </si>
+  <si>
+    <t>FX9</t>
+  </si>
+  <si>
+    <t>FX10</t>
+  </si>
+  <si>
+    <t>FX11</t>
+  </si>
+  <si>
+    <t>FX12</t>
+  </si>
+  <si>
+    <t>FX13</t>
+  </si>
+  <si>
+    <t>FS7</t>
+  </si>
+  <si>
+    <t>FS8</t>
+  </si>
+  <si>
+    <t>FS9</t>
+  </si>
+  <si>
+    <t>FS10</t>
+  </si>
+  <si>
+    <t>FS11</t>
+  </si>
+  <si>
+    <t>FS12</t>
+  </si>
+  <si>
+    <t>FS13</t>
+  </si>
+  <si>
+    <t>FS14</t>
   </si>
 </sst>
 </file>
@@ -313,7 +406,10 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -588,7 +684,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:F32" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:F32" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:F32" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{377E1240-9D46-430C-803F-4C08BD63303F}" name="Enlace" dataCellStyle="Hipervínculo"/>
@@ -596,7 +692,7 @@
     <tableColumn id="3" xr3:uid="{6C7078F4-6973-409E-B572-0FE355E1A626}" name="Marca"/>
     <tableColumn id="4" xr3:uid="{8115CCF5-4C7A-4227-90FA-D41A410A4833}" name="Modelo"/>
     <tableColumn id="5" xr3:uid="{F4F4B18E-B1F0-473E-AB7B-805E74619B4C}" name="Precio"/>
-    <tableColumn id="6" xr3:uid="{EE9A1EB6-30CC-48F5-816C-80D20CB21E97}" name="Código"/>
+    <tableColumn id="7" xr3:uid="{CB656037-B96E-4BE9-B249-FA47084BC236}" name="Código " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -921,13 +1017,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8500B94C-5AFD-412C-8663-C5BE5B0FA223}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="26.21875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -947,7 +1044,7 @@
         <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -966,6 +1063,9 @@
       <c r="E2">
         <v>1899900</v>
       </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -983,6 +1083,9 @@
       <c r="E3">
         <v>1449900</v>
       </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1000,6 +1103,9 @@
       <c r="E4" s="5">
         <v>2199900</v>
       </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1017,6 +1123,9 @@
       <c r="E5" s="5">
         <v>2199900</v>
       </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1034,6 +1143,9 @@
       <c r="E6" s="5">
         <v>3099700</v>
       </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1051,6 +1163,9 @@
       <c r="E7">
         <v>600000</v>
       </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1068,6 +1183,9 @@
       <c r="E8">
         <v>600000</v>
       </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1085,6 +1203,9 @@
       <c r="E9" s="5">
         <v>879900</v>
       </c>
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1102,6 +1223,9 @@
       <c r="E10" s="5">
         <v>879900</v>
       </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1119,6 +1243,9 @@
       <c r="E11" s="5">
         <v>949900</v>
       </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1136,6 +1263,9 @@
       <c r="E12" s="5">
         <v>1299900</v>
       </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1153,6 +1283,9 @@
       <c r="E13" s="5">
         <v>1079900</v>
       </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -1170,6 +1303,9 @@
       <c r="E14" s="5">
         <v>669900</v>
       </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -1187,6 +1323,9 @@
       <c r="E15" s="5">
         <v>2499900</v>
       </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -1204,8 +1343,11 @@
       <c r="E16" s="5">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -1216,13 +1358,16 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="5">
         <v>699900</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -1233,13 +1378,16 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="5">
         <v>612900</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1250,13 +1398,16 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="5">
         <v>599900</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1267,13 +1418,16 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5">
         <v>612900</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1289,10 +1443,13 @@
       <c r="E21" s="5">
         <v>1235000</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1306,10 +1463,13 @@
       <c r="E22" s="5">
         <v>1199900</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -1318,15 +1478,18 @@
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="5">
         <v>969900</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -1335,15 +1498,18 @@
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="5">
         <v>1299900</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -1352,15 +1518,18 @@
         <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="5">
         <v>449900</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1369,15 +1538,18 @@
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="5">
         <v>7500000</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -1386,15 +1558,18 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="5">
         <v>7500000</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1403,78 +1578,93 @@
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="5">
         <v>7499990</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
         <v>57</v>
       </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
-        <v>58</v>
-      </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" s="5">
         <v>2799900</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" s="5">
         <v>3759900</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="5">
         <v>3199900</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
         <v>65</v>
-      </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" t="s">
-        <v>66</v>
       </c>
       <c r="E32" s="5">
         <v>2549900</v>
+      </c>
+      <c r="F32" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
archivo csv de falabella creado
</commit_message>
<xml_diff>
--- a/Webscrapping/Fuentes de datos Web Scrapping.xlsx
+++ b/Webscrapping/Fuentes de datos Web Scrapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto Web Scrapping\Webscrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BF80E6-5E20-49C5-BE60-23C4170229D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ADEBFF-E4F2-4CB2-BD8C-37FCDBCE4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6468" yWindow="12" windowWidth="16560" windowHeight="12216" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -550,13 +550,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -834,7 +838,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:G49" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:G49" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:G49" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
     <sortCondition ref="C1:C49"/>
@@ -845,8 +849,8 @@
     <tableColumn id="3" xr3:uid="{6C7078F4-6973-409E-B572-0FE355E1A626}" name="Marca"/>
     <tableColumn id="4" xr3:uid="{8115CCF5-4C7A-4227-90FA-D41A410A4833}" name="Modelo"/>
     <tableColumn id="6" xr3:uid="{61CD5531-4759-4B04-B72E-F44DAA07D8FA}" name="Modelo estandar"/>
-    <tableColumn id="5" xr3:uid="{F4F4B18E-B1F0-473E-AB7B-805E74619B4C}" name="Precio"/>
-    <tableColumn id="7" xr3:uid="{CB656037-B96E-4BE9-B249-FA47084BC236}" name="Código " dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{F4F4B18E-B1F0-473E-AB7B-805E74619B4C}" name="Precio" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{CB656037-B96E-4BE9-B249-FA47084BC236}" name="Código " dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1171,15 +1175,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8500B94C-5AFD-412C-8663-C5BE5B0FA223}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="30.88671875" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="6" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1199,7 +1203,7 @@
       <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1222,7 +1226,7 @@
       <c r="E2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>2799900</v>
       </c>
       <c r="G2" t="s">
@@ -1245,7 +1249,7 @@
       <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>3759900</v>
       </c>
       <c r="G3" t="s">
@@ -1268,7 +1272,7 @@
       <c r="E4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>3199900</v>
       </c>
       <c r="G4" t="s">
@@ -1291,7 +1295,7 @@
       <c r="E5" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>2549900</v>
       </c>
       <c r="G5" t="s">
@@ -1312,7 +1316,7 @@
       <c r="E6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>1754910</v>
       </c>
       <c r="G6" t="s">
@@ -1333,7 +1337,7 @@
       <c r="E7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>2499900</v>
       </c>
       <c r="G7" t="s">
@@ -1354,7 +1358,7 @@
       <c r="E8" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>3169000</v>
       </c>
       <c r="G8" t="s">
@@ -1375,7 +1379,7 @@
       <c r="E9" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6">
         <v>3217900</v>
       </c>
       <c r="G9" t="s">
@@ -1398,7 +1402,7 @@
       <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>2499900</v>
       </c>
       <c r="G10" t="s">
@@ -1421,7 +1425,7 @@
       <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <v>2000000</v>
       </c>
       <c r="G11" t="s">
@@ -1444,7 +1448,7 @@
       <c r="E12" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <v>699900</v>
       </c>
       <c r="G12" t="s">
@@ -1467,7 +1471,7 @@
       <c r="E13" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="6">
         <v>612900</v>
       </c>
       <c r="G13" t="s">
@@ -1490,7 +1494,7 @@
       <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <v>599900</v>
       </c>
       <c r="G14" t="s">
@@ -1513,7 +1517,7 @@
       <c r="E15" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <v>612900</v>
       </c>
       <c r="G15" t="s">
@@ -1536,7 +1540,7 @@
       <c r="E16" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>1235000</v>
       </c>
       <c r="G16" t="s">
@@ -1559,7 +1563,7 @@
       <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="6">
         <v>1199900</v>
       </c>
       <c r="G17" t="s">
@@ -1582,7 +1586,7 @@
       <c r="E18" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6">
         <v>969900</v>
       </c>
       <c r="G18" t="s">
@@ -1605,7 +1609,7 @@
       <c r="E19" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6">
         <v>1299900</v>
       </c>
       <c r="G19" t="s">
@@ -1628,7 +1632,7 @@
       <c r="E20" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="6">
         <v>449900</v>
       </c>
       <c r="G20" t="s">
@@ -1651,7 +1655,7 @@
       <c r="E21" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="6">
         <v>7500000</v>
       </c>
       <c r="G21" t="s">
@@ -1674,7 +1678,7 @@
       <c r="E22" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="6">
         <v>7500000</v>
       </c>
       <c r="G22" t="s">
@@ -1697,7 +1701,7 @@
       <c r="E23" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6">
         <v>7499990</v>
       </c>
       <c r="G23" t="s">
@@ -1718,7 +1722,7 @@
       <c r="E24" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="6">
         <v>431433</v>
       </c>
       <c r="G24" t="s">
@@ -1739,7 +1743,7 @@
       <c r="E25" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="6">
         <v>599900</v>
       </c>
       <c r="G25" t="s">
@@ -1760,7 +1764,7 @@
       <c r="E26" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="6">
         <v>849900</v>
       </c>
       <c r="G26" t="s">
@@ -1781,7 +1785,7 @@
       <c r="E27" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="6">
         <v>949900</v>
       </c>
       <c r="G27" t="s">
@@ -1802,7 +1806,7 @@
       <c r="E28" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="6">
         <v>1387900</v>
       </c>
       <c r="G28" t="s">
@@ -1823,7 +1827,7 @@
       <c r="E29" t="s">
         <v>133</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="6">
         <v>4349900</v>
       </c>
       <c r="G29" t="s">
@@ -1844,7 +1848,7 @@
       <c r="E30" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="6">
         <v>4529900</v>
       </c>
       <c r="G30" t="s">
@@ -1867,7 +1871,7 @@
       <c r="E31" t="s">
         <v>38</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="6">
         <v>1899900</v>
       </c>
       <c r="G31" t="s">
@@ -1890,7 +1894,7 @@
       <c r="E32" t="s">
         <v>38</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="6">
         <v>1449900</v>
       </c>
       <c r="G32" t="s">
@@ -1913,7 +1917,7 @@
       <c r="E33" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="6">
         <v>2199900</v>
       </c>
       <c r="G33" t="s">
@@ -1936,7 +1940,7 @@
       <c r="E34" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="6">
         <v>2199900</v>
       </c>
       <c r="G34" t="s">
@@ -1959,7 +1963,7 @@
       <c r="E35" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="6">
         <v>3099700</v>
       </c>
       <c r="G35" t="s">
@@ -1982,7 +1986,7 @@
       <c r="E36" t="s">
         <v>40</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="6">
         <v>600000</v>
       </c>
       <c r="G36" t="s">
@@ -2005,7 +2009,7 @@
       <c r="E37" t="s">
         <v>40</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="6">
         <v>600000</v>
       </c>
       <c r="G37" t="s">
@@ -2028,7 +2032,7 @@
       <c r="E38" t="s">
         <v>41</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="6">
         <v>879900</v>
       </c>
       <c r="G38" t="s">
@@ -2051,7 +2055,7 @@
       <c r="E39" t="s">
         <v>42</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="6">
         <v>879900</v>
       </c>
       <c r="G39" t="s">
@@ -2074,7 +2078,7 @@
       <c r="E40" t="s">
         <v>41</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="6">
         <v>949900</v>
       </c>
       <c r="G40" t="s">
@@ -2097,7 +2101,7 @@
       <c r="E41" t="s">
         <v>41</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="6">
         <v>1299900</v>
       </c>
       <c r="G41" t="s">
@@ -2120,7 +2124,7 @@
       <c r="E42" t="s">
         <v>43</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="6">
         <v>1079900</v>
       </c>
       <c r="G42" t="s">
@@ -2143,7 +2147,7 @@
       <c r="E43" t="s">
         <v>43</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="6">
         <v>669900</v>
       </c>
       <c r="G43" t="s">
@@ -2164,7 +2168,7 @@
       <c r="E44" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="6">
         <v>1304900</v>
       </c>
       <c r="G44" t="s">
@@ -2185,7 +2189,7 @@
       <c r="E45" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="6">
         <v>479940</v>
       </c>
       <c r="G45" t="s">
@@ -2206,7 +2210,7 @@
       <c r="E46" t="s">
         <v>24</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="6">
         <v>299900</v>
       </c>
       <c r="G46" t="s">
@@ -2227,7 +2231,7 @@
       <c r="E47" t="s">
         <v>43</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="6">
         <v>617900</v>
       </c>
       <c r="G47" t="s">
@@ -2248,7 +2252,7 @@
       <c r="E48" t="s">
         <v>41</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="6">
         <v>890946</v>
       </c>
       <c r="G48" t="s">
@@ -2269,7 +2273,7 @@
       <c r="E49" t="s">
         <v>41</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="6">
         <v>1619940</v>
       </c>
       <c r="G49" t="s">

</xml_diff>

<commit_message>
actualización codigo principal con subida de las tres tablas a SQL
</commit_message>
<xml_diff>
--- a/Webscrapping/Fuentes de datos Web Scrapping.xlsx
+++ b/Webscrapping/Fuentes de datos Web Scrapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto Web Scrapping\Webscrapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Scrapping Sentimientos Project\Project_repository\Webscrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19757130-D948-4EF1-B0C0-882BE3BD079B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA51E5A-B2F0-40AC-BB32-326631731C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -285,9 +285,6 @@
     <t>FI4</t>
   </si>
   <si>
-    <t xml:space="preserve">Código </t>
-  </si>
-  <si>
     <t>FX6</t>
   </si>
   <si>
@@ -484,6 +481,9 @@
   </si>
   <si>
     <t>MX19</t>
+  </si>
+  <si>
+    <t>Código</t>
   </si>
 </sst>
 </file>
@@ -839,7 +839,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:G49" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:G49" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
     <sortCondition ref="C1:C49"/>
   </sortState>
@@ -850,7 +849,7 @@
     <tableColumn id="4" xr3:uid="{8115CCF5-4C7A-4227-90FA-D41A410A4833}" name="Modelo"/>
     <tableColumn id="6" xr3:uid="{61CD5531-4759-4B04-B72E-F44DAA07D8FA}" name="Modelo estandar"/>
     <tableColumn id="5" xr3:uid="{F4F4B18E-B1F0-473E-AB7B-805E74619B4C}" name="Precio" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{CB656037-B96E-4BE9-B249-FA47084BC236}" name="Código " dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{CB656037-B96E-4BE9-B249-FA47084BC236}" name="Código" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1176,7 +1175,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,13 +1200,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1221,7 +1220,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
         <v>59</v>
@@ -1244,7 +1243,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
         <v>62</v>
@@ -1267,7 +1266,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
         <v>61</v>
@@ -1290,7 +1289,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
         <v>65</v>
@@ -1305,13 +1304,13 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
         <v>65</v>
@@ -1320,19 +1319,19 @@
         <v>1754910</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
         <v>59</v>
@@ -1341,19 +1340,19 @@
         <v>2499900</v>
       </c>
       <c r="G7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
         <v>61</v>
@@ -1362,19 +1361,19 @@
         <v>3169000</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
         <v>62</v>
@@ -1383,7 +1382,7 @@
         <v>3217900</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1397,7 +1396,7 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -1420,7 +1419,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -1535,7 +1534,7 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
         <v>44</v>
@@ -1544,7 +1543,7 @@
         <v>1235000</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1558,7 +1557,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
         <v>44</v>
@@ -1567,7 +1566,7 @@
         <v>1199900</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1581,7 +1580,7 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E18" t="s">
         <v>49</v>
@@ -1590,7 +1589,7 @@
         <v>969900</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1604,7 +1603,7 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E19" t="s">
         <v>49</v>
@@ -1613,7 +1612,7 @@
         <v>1299900</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1627,7 +1626,7 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
         <v>52</v>
@@ -1636,7 +1635,7 @@
         <v>449900</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1650,7 +1649,7 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s">
         <v>58</v>
@@ -1659,7 +1658,7 @@
         <v>7500000</v>
       </c>
       <c r="G21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1673,7 +1672,7 @@
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s">
         <v>58</v>
@@ -1682,7 +1681,7 @@
         <v>7500000</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1696,7 +1695,7 @@
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
         <v>58</v>
@@ -1705,19 +1704,19 @@
         <v>7499990</v>
       </c>
       <c r="G23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" t="s">
         <v>52</v>
@@ -1726,19 +1725,19 @@
         <v>431433</v>
       </c>
       <c r="G24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
@@ -1747,19 +1746,19 @@
         <v>599900</v>
       </c>
       <c r="G25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E26" t="s">
         <v>44</v>
@@ -1768,19 +1767,19 @@
         <v>849900</v>
       </c>
       <c r="G26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" t="s">
         <v>49</v>
@@ -1789,19 +1788,19 @@
         <v>949900</v>
       </c>
       <c r="G27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
@@ -1810,40 +1809,40 @@
         <v>1387900</v>
       </c>
       <c r="G28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F29" s="6">
         <v>4349900</v>
       </c>
       <c r="G29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" t="s">
         <v>58</v>
@@ -1852,7 +1851,7 @@
         <v>4529900</v>
       </c>
       <c r="G30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1912,7 +1911,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E33" t="s">
         <v>39</v>
@@ -1935,7 +1934,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E34" t="s">
         <v>39</v>
@@ -1958,7 +1957,7 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E35" t="s">
         <v>39</v>
@@ -1981,7 +1980,7 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E36" t="s">
         <v>40</v>
@@ -1990,7 +1989,7 @@
         <v>600000</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2004,7 +2003,7 @@
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E37" t="s">
         <v>40</v>
@@ -2013,7 +2012,7 @@
         <v>600000</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2027,7 +2026,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
         <v>41</v>
@@ -2036,7 +2035,7 @@
         <v>879900</v>
       </c>
       <c r="G38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2050,7 +2049,7 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E39" t="s">
         <v>42</v>
@@ -2059,7 +2058,7 @@
         <v>879900</v>
       </c>
       <c r="G39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2073,7 +2072,7 @@
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E40" t="s">
         <v>41</v>
@@ -2082,7 +2081,7 @@
         <v>949900</v>
       </c>
       <c r="G40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2096,7 +2095,7 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E41" t="s">
         <v>41</v>
@@ -2105,7 +2104,7 @@
         <v>1299900</v>
       </c>
       <c r="G41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2128,7 +2127,7 @@
         <v>1079900</v>
       </c>
       <c r="G42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2151,19 +2150,19 @@
         <v>669900</v>
       </c>
       <c r="G43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E44" t="s">
         <v>38</v>
@@ -2172,19 +2171,19 @@
         <v>1304900</v>
       </c>
       <c r="G44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E45" t="s">
         <v>40</v>
@@ -2193,19 +2192,19 @@
         <v>479940</v>
       </c>
       <c r="G45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
         <v>24</v>
@@ -2214,19 +2213,19 @@
         <v>299900</v>
       </c>
       <c r="G46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
         <v>43</v>
@@ -2235,19 +2234,19 @@
         <v>617900</v>
       </c>
       <c r="G47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E48" t="s">
         <v>41</v>
@@ -2256,19 +2255,19 @@
         <v>890946</v>
       </c>
       <c r="G48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E49" t="s">
         <v>41</v>
@@ -2277,7 +2276,7 @@
         <v>1619940</v>
       </c>
       <c r="G49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion primer query de SQL con unificacionde la informacion
</commit_message>
<xml_diff>
--- a/Webscrapping/Fuentes de datos Web Scrapping.xlsx
+++ b/Webscrapping/Fuentes de datos Web Scrapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Scrapping Sentimientos Project\Project_repository\Webscrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA51E5A-B2F0-40AC-BB32-326631731C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD702DC-8EFF-44BE-BF3A-0C0460AEDE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6A2C7A7-BBC6-4ECF-8AEA-C7202E7C2CBA}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="147">
   <si>
     <t>Marca</t>
   </si>
@@ -165,15 +165,9 @@
     <t xml:space="preserve">Xiaomi Redmi 13C </t>
   </si>
   <si>
-    <t xml:space="preserve">Xiaomi Redmi Note 13 Pro </t>
-  </si>
-  <si>
     <t>Xiaomi Redmi Note 13 Pro</t>
   </si>
   <si>
-    <t xml:space="preserve">Xiaomi Redmi Note 13 </t>
-  </si>
-  <si>
     <t>Samsung Galaxy A25</t>
   </si>
   <si>
@@ -484,6 +478,9 @@
   </si>
   <si>
     <t>Código</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 13</t>
   </si>
 </sst>
 </file>
@@ -840,7 +837,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48165FE3-C1EF-4C38-8034-78FB41426AB6}" name="Tabla1" displayName="Tabla1" ref="A1:G49" totalsRowShown="0" headerRowDxfId="2">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
-    <sortCondition ref="C1:C49"/>
+    <sortCondition ref="E1:E49"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{377E1240-9D46-430C-803F-4C08BD63303F}" name="Enlace" dataCellStyle="Hipervínculo"/>
@@ -1174,14 +1171,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8500B94C-5AFD-412C-8663-C5BE5B0FA223}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="30.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" style="6" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
@@ -1200,194 +1195,194 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F2" s="6">
-        <v>2799900</v>
+        <v>2549900</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F3" s="6">
-        <v>3759900</v>
+        <v>1754910</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>118</v>
       </c>
       <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2799900</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="6">
+        <v>2499900</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="6">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="6">
         <v>3199900</v>
       </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2549900</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1754910</v>
-      </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
         <v>59</v>
       </c>
       <c r="F7" s="6">
-        <v>2499900</v>
+        <v>3169000</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="6">
-        <v>3169000</v>
+        <v>3759900</v>
       </c>
       <c r="G8" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" s="6">
         <v>3217900</v>
       </c>
       <c r="G9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -1396,39 +1391,37 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F10" s="6">
-        <v>2499900</v>
+        <v>449900</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F11" s="6">
-        <v>2000000</v>
+        <v>431433</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1445,13 +1438,13 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F12" s="6">
         <v>699900</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1468,13 +1461,13 @@
         <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F13" s="6">
         <v>612900</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1491,13 +1484,13 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F14" s="6">
         <v>599900</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1514,41 +1507,39 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F15" s="6">
         <v>612900</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>44</v>
       </c>
       <c r="F16" s="6">
-        <v>1235000</v>
+        <v>599900</v>
       </c>
       <c r="G16" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -1557,21 +1548,21 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F17" s="6">
-        <v>1199900</v>
+        <v>1235000</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -1580,44 +1571,42 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F18" s="6">
-        <v>969900</v>
+        <v>1199900</v>
       </c>
       <c r="G18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F19" s="6">
-        <v>1299900</v>
+        <v>849900</v>
       </c>
       <c r="G19" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1626,21 +1615,21 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F20" s="6">
-        <v>449900</v>
+        <v>969900</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1649,44 +1638,42 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F21" s="6">
-        <v>7500000</v>
+        <v>1299900</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F22" s="6">
-        <v>7500000</v>
+        <v>949900</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -1695,43 +1682,45 @@
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="F23" s="6">
-        <v>7499990</v>
+        <v>2499900</v>
       </c>
       <c r="G23" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B24" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="F24" s="6">
-        <v>431433</v>
+        <v>2000000</v>
       </c>
       <c r="G24" t="s">
-        <v>134</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -1740,19 +1729,19 @@
         <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F25" s="6">
-        <v>599900</v>
+        <v>1387900</v>
       </c>
       <c r="G25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
@@ -1761,97 +1750,103 @@
         <v>103</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="F26" s="6">
-        <v>849900</v>
+        <v>4349900</v>
       </c>
       <c r="G26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F27" s="6">
-        <v>949900</v>
+        <v>7500000</v>
       </c>
       <c r="G27" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F28" s="6">
-        <v>1387900</v>
+        <v>7500000</v>
       </c>
       <c r="G28" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
+        <v>56</v>
       </c>
       <c r="F29" s="6">
-        <v>4349900</v>
+        <v>7499990</v>
       </c>
       <c r="G29" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F30" s="6">
         <v>4529900</v>
       </c>
       <c r="G30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1874,7 +1869,7 @@
         <v>1899900</v>
       </c>
       <c r="G31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1897,35 +1892,33 @@
         <v>1449900</v>
       </c>
       <c r="G32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A33" s="2"/>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="E33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F33" s="6">
-        <v>2199900</v>
+        <v>1304900</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -1937,18 +1930,18 @@
         <v>127</v>
       </c>
       <c r="E34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F34" s="6">
-        <v>2199900</v>
+        <v>600000</v>
       </c>
       <c r="G34" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -1960,64 +1953,60 @@
         <v>127</v>
       </c>
       <c r="E35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F35" s="6">
-        <v>3099700</v>
+        <v>600000</v>
       </c>
       <c r="G35" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A36" s="2"/>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="E36" t="s">
         <v>40</v>
       </c>
       <c r="F36" s="6">
-        <v>600000</v>
+        <v>479940</v>
       </c>
       <c r="G36" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A37" s="2"/>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F37" s="6">
-        <v>600000</v>
+        <v>299900</v>
       </c>
       <c r="G37" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -2026,21 +2015,21 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="F38" s="6">
-        <v>879900</v>
+        <v>1079900</v>
       </c>
       <c r="G38" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -2049,44 +2038,42 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="F39" s="6">
-        <v>879900</v>
+        <v>669900</v>
       </c>
       <c r="G39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A40" s="2"/>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="E40" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="F40" s="6">
-        <v>949900</v>
+        <v>617900</v>
       </c>
       <c r="G40" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -2095,21 +2082,21 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E41" t="s">
         <v>41</v>
       </c>
       <c r="F41" s="6">
-        <v>1299900</v>
+        <v>879900</v>
       </c>
       <c r="G41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -2118,21 +2105,21 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F42" s="6">
-        <v>1079900</v>
+        <v>879900</v>
       </c>
       <c r="G42" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -2141,142 +2128,150 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="E43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F43" s="6">
-        <v>669900</v>
+        <v>949900</v>
       </c>
       <c r="G43" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F44" s="6">
-        <v>1304900</v>
+        <v>1299900</v>
       </c>
       <c r="G44" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F45" s="6">
-        <v>479940</v>
+        <v>890946</v>
       </c>
       <c r="G45" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F46" s="6">
-        <v>299900</v>
+        <v>1619940</v>
       </c>
       <c r="G46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
+      <c r="A47" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F47" s="6">
-        <v>617900</v>
+        <v>2199900</v>
       </c>
       <c r="G47" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
+      <c r="A48" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B48" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="E48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F48" s="6">
-        <v>890946</v>
+        <v>2199900</v>
       </c>
       <c r="G48" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B49" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F49" s="6">
-        <v>1619940</v>
+        <v>3099700</v>
       </c>
       <c r="G49" t="s">
-        <v>146</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2284,35 +2279,35 @@
   <hyperlinks>
     <hyperlink ref="A31" r:id="rId1" xr:uid="{E7F26927-24E0-4939-9FA8-B4BC57A735B4}"/>
     <hyperlink ref="A32" r:id="rId2" xr:uid="{A0E0A9F9-898D-4542-9E87-2B280EB717F0}"/>
-    <hyperlink ref="A33" r:id="rId3" xr:uid="{84738B62-D2DF-4836-B01E-9104A1CF7953}"/>
-    <hyperlink ref="A34" r:id="rId4" xr:uid="{48958B1B-E98E-4FEC-B879-A57EF0B2D4A3}"/>
-    <hyperlink ref="A35" r:id="rId5" xr:uid="{AC356D92-261D-471D-BF1A-4A7CFC69E00A}"/>
-    <hyperlink ref="A36" r:id="rId6" xr:uid="{CBB60518-4888-4CBA-8109-CE0D52741AAF}"/>
-    <hyperlink ref="A37" r:id="rId7" xr:uid="{A47B20A5-058F-4C51-9864-56310EB8B5B4}"/>
-    <hyperlink ref="A38" r:id="rId8" xr:uid="{9F714AB6-F716-4291-B6B2-D763E3929C73}"/>
-    <hyperlink ref="A39" r:id="rId9" xr:uid="{8A8D875E-B42F-41A3-9636-08E530B6FA82}"/>
-    <hyperlink ref="A40" r:id="rId10" xr:uid="{3AE62428-39FD-4E3D-BF85-36D177A74792}"/>
-    <hyperlink ref="A41" r:id="rId11" xr:uid="{090E4DF1-D4C3-40CD-921A-453EF53FD8C2}"/>
-    <hyperlink ref="A42" r:id="rId12" xr:uid="{9B0B241E-2775-4049-9C58-DFE1303229AC}"/>
-    <hyperlink ref="A43" r:id="rId13" xr:uid="{B4E566C2-E281-4E14-85EF-0017A6237ED7}"/>
-    <hyperlink ref="A11" r:id="rId14" xr:uid="{7D27F7E4-07C5-4486-A09D-914A0DB4CBE6}"/>
+    <hyperlink ref="A47" r:id="rId3" xr:uid="{84738B62-D2DF-4836-B01E-9104A1CF7953}"/>
+    <hyperlink ref="A48" r:id="rId4" xr:uid="{48958B1B-E98E-4FEC-B879-A57EF0B2D4A3}"/>
+    <hyperlink ref="A49" r:id="rId5" xr:uid="{AC356D92-261D-471D-BF1A-4A7CFC69E00A}"/>
+    <hyperlink ref="A34" r:id="rId6" xr:uid="{CBB60518-4888-4CBA-8109-CE0D52741AAF}"/>
+    <hyperlink ref="A35" r:id="rId7" xr:uid="{A47B20A5-058F-4C51-9864-56310EB8B5B4}"/>
+    <hyperlink ref="A42" r:id="rId8" xr:uid="{9F714AB6-F716-4291-B6B2-D763E3929C73}"/>
+    <hyperlink ref="A41" r:id="rId9" xr:uid="{8A8D875E-B42F-41A3-9636-08E530B6FA82}"/>
+    <hyperlink ref="A43" r:id="rId10" xr:uid="{3AE62428-39FD-4E3D-BF85-36D177A74792}"/>
+    <hyperlink ref="A44" r:id="rId11" xr:uid="{090E4DF1-D4C3-40CD-921A-453EF53FD8C2}"/>
+    <hyperlink ref="A38" r:id="rId12" xr:uid="{9B0B241E-2775-4049-9C58-DFE1303229AC}"/>
+    <hyperlink ref="A39" r:id="rId13" xr:uid="{B4E566C2-E281-4E14-85EF-0017A6237ED7}"/>
+    <hyperlink ref="A24" r:id="rId14" xr:uid="{7D27F7E4-07C5-4486-A09D-914A0DB4CBE6}"/>
     <hyperlink ref="A12" r:id="rId15" xr:uid="{D1B444DD-33A9-498D-B3A9-9089A761661B}"/>
     <hyperlink ref="A13" r:id="rId16" xr:uid="{3EAEB76C-F201-47A4-8325-1248E769E333}"/>
     <hyperlink ref="A14" r:id="rId17" xr:uid="{98A5927C-997C-4285-9C5C-07EFD99C107A}"/>
     <hyperlink ref="A15" r:id="rId18" xr:uid="{8CDECC3D-DA84-4D6E-B8CD-6915D1937740}"/>
-    <hyperlink ref="A16" r:id="rId19" xr:uid="{2D2B0672-EC1C-4184-8E98-33DEFC7FCED5}"/>
-    <hyperlink ref="A10" r:id="rId20" xr:uid="{BDDB22E4-BCCD-43FD-B377-4C9ACC77A8DC}"/>
-    <hyperlink ref="A17" r:id="rId21" xr:uid="{82270B06-9912-4791-97A1-C0EDDFBB60DF}"/>
-    <hyperlink ref="A18" r:id="rId22" xr:uid="{F2382336-A0CF-4933-93E7-92BC97C63F56}"/>
-    <hyperlink ref="A19" r:id="rId23" xr:uid="{EBE7E398-1E23-4786-83D7-6B064E34B571}"/>
-    <hyperlink ref="A20" r:id="rId24" xr:uid="{3FFA4EF1-06AB-42C1-BE08-0BC48AA24A12}"/>
-    <hyperlink ref="A21" r:id="rId25" xr:uid="{7E4554B0-87E3-4A1E-BDFF-155340CBA46C}"/>
-    <hyperlink ref="A22" r:id="rId26" xr:uid="{AE68D55E-9520-48FB-84C6-3EFEDBB73037}"/>
-    <hyperlink ref="A23" r:id="rId27" xr:uid="{7FA50F87-3340-48F3-B2EF-C56E5709038E}"/>
-    <hyperlink ref="A2" r:id="rId28" xr:uid="{0A62AC0B-84C1-43DA-86E7-84765FF424BF}"/>
-    <hyperlink ref="A3" r:id="rId29" xr:uid="{426D4B11-FA7E-4CD4-8D0B-95237D52D2DE}"/>
-    <hyperlink ref="A4" r:id="rId30" xr:uid="{354F6FE1-0A02-4D1D-A1B5-FDB8EED61F95}"/>
-    <hyperlink ref="A5" r:id="rId31" xr:uid="{662B402D-4086-4B7C-9655-FEA5DE28A50D}"/>
+    <hyperlink ref="A17" r:id="rId19" xr:uid="{2D2B0672-EC1C-4184-8E98-33DEFC7FCED5}"/>
+    <hyperlink ref="A23" r:id="rId20" xr:uid="{BDDB22E4-BCCD-43FD-B377-4C9ACC77A8DC}"/>
+    <hyperlink ref="A18" r:id="rId21" xr:uid="{82270B06-9912-4791-97A1-C0EDDFBB60DF}"/>
+    <hyperlink ref="A20" r:id="rId22" xr:uid="{F2382336-A0CF-4933-93E7-92BC97C63F56}"/>
+    <hyperlink ref="A21" r:id="rId23" xr:uid="{EBE7E398-1E23-4786-83D7-6B064E34B571}"/>
+    <hyperlink ref="A10" r:id="rId24" xr:uid="{3FFA4EF1-06AB-42C1-BE08-0BC48AA24A12}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{7E4554B0-87E3-4A1E-BDFF-155340CBA46C}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{AE68D55E-9520-48FB-84C6-3EFEDBB73037}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{7FA50F87-3340-48F3-B2EF-C56E5709038E}"/>
+    <hyperlink ref="A4" r:id="rId28" xr:uid="{0A62AC0B-84C1-43DA-86E7-84765FF424BF}"/>
+    <hyperlink ref="A8" r:id="rId29" xr:uid="{426D4B11-FA7E-4CD4-8D0B-95237D52D2DE}"/>
+    <hyperlink ref="A6" r:id="rId30" xr:uid="{354F6FE1-0A02-4D1D-A1B5-FDB8EED61F95}"/>
+    <hyperlink ref="A2" r:id="rId31" xr:uid="{662B402D-4086-4B7C-9655-FEA5DE28A50D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>